<commit_message>
readme work, reran outputs
</commit_message>
<xml_diff>
--- a/data/simon_mastersnew.xlsx
+++ b/data/simon_mastersnew.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B2D1C5-4359-4278-BD1F-E9DDECD8F373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>program_run?</t>
   </si>
@@ -179,6 +173,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
   <si>
     <t>2020-07-30</t>
@@ -238,8 +235,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,14 +299,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -356,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,27 +377,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -440,24 +411,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -633,16 +586,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,24 +751,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
         <v>52</v>
@@ -832,39 +783,39 @@
         <v>34.5</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T2">
-        <v>0.98179678992434138</v>
+        <v>0.9817967899243414</v>
       </c>
       <c r="U2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="V2">
-        <v>1.008573325607265E-2</v>
+        <v>0.01008573325607265</v>
       </c>
       <c r="Y2">
-        <v>0.97659884636276562</v>
+        <v>0.9765988463627656</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52">
       <c r="A3" t="s">
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
         <v>52</v>
@@ -879,45 +830,45 @@
         <v>34.5</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R3">
-        <v>171.28104068040801</v>
+        <v>171.281040680408</v>
       </c>
       <c r="S3">
-        <v>1.6932982948525639E-2</v>
+        <v>0.01693298294852564</v>
       </c>
       <c r="T3">
-        <v>0.95643911455691333</v>
+        <v>0.9564391145569133</v>
       </c>
       <c r="V3">
-        <v>1.8126592925987631E-2</v>
+        <v>0.01812659292598763</v>
       </c>
       <c r="Y3">
-        <v>0.97659884636276562</v>
+        <v>0.9765988463627656</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" t="s">
-        <v>66</v>
-      </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -929,27 +880,27 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52">
       <c r="A5" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -961,24 +912,24 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J6">
         <v>0</v>

</xml_diff>

<commit_message>
program_run = n for times outside lgr data
</commit_message>
<xml_diff>
--- a/data/simon_mastersnew.xlsx
+++ b/data/simon_mastersnew.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
     <t>program_run?</t>
   </si>
@@ -181,7 +181,7 @@
     <t>y</t>
   </si>
   <si>
-    <t>p</t>
+    <t>n</t>
   </si>
   <si>
     <t>2020-07-30</t>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>chamber</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>2020_07_30_17h12m20s_vault-lake_bucket_CO2</t>
@@ -804,7 +801,7 @@
         <v>34.5</v>
       </c>
       <c r="W2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -842,7 +839,7 @@
         <v>34.5</v>
       </c>
       <c r="O3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V3">
         <v>0.9817967899243414</v>
@@ -889,7 +886,7 @@
         <v>34.5</v>
       </c>
       <c r="O4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T4">
         <v>171.281040680408</v>
@@ -927,7 +924,7 @@
         <v>71</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -962,7 +959,7 @@
         <v>71</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -975,6 +972,9 @@
       </c>
     </row>
     <row r="7" spans="1:54">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -994,7 +994,7 @@
         <v>71</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="L7">
         <v>0</v>

</xml_diff>

<commit_message>
records r_2 values for rejected data
</commit_message>
<xml_diff>
--- a/data/simon_mastersnew.xlsx
+++ b/data/simon_mastersnew.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>program_run?</t>
   </si>
@@ -58,6 +58,9 @@
     <t>exposed_height(cm)</t>
   </si>
   <si>
+    <t>min sample length</t>
+  </si>
+  <si>
     <t>Sample ID</t>
   </si>
   <si>
@@ -226,13 +229,13 @@
     <t>21:15:30</t>
   </si>
   <si>
-    <t>bucket</t>
+    <t>bucket_sediment</t>
   </si>
   <si>
     <t>chamber</t>
   </si>
   <si>
-    <t>2020_07_30_17h12m20s_vault-lake_bucket_CO2</t>
+    <t>2020_07_30_17h12m20s_vault-lake_bucket_sediment_CO2</t>
   </si>
   <si>
     <t>2020_07_30_18h12m20s_vault-lake_chamber_CH4</t>
@@ -596,13 +599,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:55">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,31 +768,34 @@
       <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:55">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -800,34 +806,40 @@
       <c r="N2">
         <v>34.5</v>
       </c>
-      <c r="W2" t="s">
-        <v>74</v>
+      <c r="O2">
+        <v>45</v>
+      </c>
+      <c r="W2">
+        <v>0.5393535609116455</v>
+      </c>
+      <c r="X2" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:55">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -838,43 +850,46 @@
       <c r="N3">
         <v>34.5</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>45</v>
+      </c>
+      <c r="P3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W3">
+        <v>0.9817967899243414</v>
+      </c>
+      <c r="Y3">
+        <v>0.01008573325607265</v>
+      </c>
+      <c r="AB3">
+        <v>0.9765988463627656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
         <v>72</v>
       </c>
-      <c r="V3">
-        <v>0.9817967899243414</v>
-      </c>
-      <c r="X3">
-        <v>0.01008573325607265</v>
-      </c>
-      <c r="AA3">
-        <v>0.9765988463627656</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" t="s">
-        <v>71</v>
-      </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -885,46 +900,49 @@
       <c r="N4">
         <v>34.5</v>
       </c>
-      <c r="O4" t="s">
-        <v>73</v>
-      </c>
-      <c r="T4">
+      <c r="O4">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>74</v>
+      </c>
+      <c r="U4">
         <v>171.281040680408</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.01693298294852564</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0.9564391145569133</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>0.9765988463627656</v>
       </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:55">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" t="s">
-        <v>55</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -935,31 +953,34 @@
       <c r="N5">
         <v>34.5</v>
       </c>
+      <c r="O5">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:55">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
         <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" t="s">
-        <v>55</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -970,31 +991,34 @@
       <c r="N6">
         <v>34.5</v>
       </c>
+      <c r="O6">
+        <v>45</v>
+      </c>
     </row>
-    <row r="7" spans="1:54">
+    <row r="7" spans="1:55">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K7" t="s">
-        <v>55</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1004,6 +1028,9 @@
       </c>
       <c r="N7">
         <v>34.5</v>
+      </c>
+      <c r="O7">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pulls r_2 values from excel sheet
</commit_message>
<xml_diff>
--- a/data/simon_mastersnew.xlsx
+++ b/data/simon_mastersnew.xlsx
@@ -857,10 +857,10 @@
         <v>73</v>
       </c>
       <c r="W3">
-        <v>0.9817967899243414</v>
+        <v>0.9851912822914085</v>
       </c>
       <c r="Y3">
-        <v>0.01008573325607265</v>
+        <v>0.01070685442323115</v>
       </c>
       <c r="AB3">
         <v>0.9765988463627656</v>
@@ -907,13 +907,13 @@
         <v>74</v>
       </c>
       <c r="U4">
-        <v>171.281040680408</v>
+        <v>186.7832931399875</v>
       </c>
       <c r="V4">
-        <v>0.01693298294852564</v>
+        <v>0.01188074390501766</v>
       </c>
       <c r="W4">
-        <v>0.9564391145569133</v>
+        <v>0.9850050806033371</v>
       </c>
       <c r="AB4">
         <v>0.9765988463627656</v>

</xml_diff>